<commit_message>
15-02-2026 ajj mai bassisc ka practuice karunga
</commit_message>
<xml_diff>
--- a/Progress Tracking.xlsx
+++ b/Progress Tracking.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA-JAVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498A043F-7868-4836-9272-A62C1A94CCDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A113270-1606-4ED6-8317-0A0E2A0E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{74DA7082-15CB-48A2-8E86-E4786E99D695}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{74DA7082-15CB-48A2-8E86-E4786E99D695}"/>
   </bookViews>
   <sheets>
     <sheet name="Self Practic" sheetId="1" r:id="rId1"/>
     <sheet name="Apna College" sheetId="2" r:id="rId2"/>
     <sheet name="Live-Session" sheetId="3" r:id="rId3"/>
+    <sheet name="Important Problem-Topic Wise" sheetId="4" r:id="rId4"/>
+    <sheet name="REACT Dev" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="112">
   <si>
     <t>Problem</t>
   </si>
@@ -277,13 +279,112 @@
   </si>
   <si>
     <t>trainne</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>STRINGS</t>
+  </si>
+  <si>
+    <t>LINKED-LIST</t>
+  </si>
+  <si>
+    <t>STACK&amp;QUEUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BINARY  TREE </t>
+  </si>
+  <si>
+    <t>BINARY SEARCH REE</t>
+  </si>
+  <si>
+    <t>Two Sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best Time to Buy &amp; Sell Stock </t>
+  </si>
+  <si>
+    <t>Maximum Subarray (kadane)</t>
+  </si>
+  <si>
+    <t>Merge intervals</t>
+  </si>
+  <si>
+    <t>3Sum</t>
+  </si>
+  <si>
+    <t>3sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product of Array Excpt  Self </t>
+  </si>
+  <si>
+    <t>Cointainer With most water</t>
+  </si>
+  <si>
+    <t>Set matrix zeroes</t>
+  </si>
+  <si>
+    <t>Rotate Array</t>
+  </si>
+  <si>
+    <t>Missing Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longest Substring Without Reapeating Character </t>
+  </si>
+  <si>
+    <t>Valid Anagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longest Palindromic Substring </t>
+  </si>
+  <si>
+    <t xml:space="preserve">String to integer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reverse words in string </t>
+  </si>
+  <si>
+    <t>valid parantheses</t>
+  </si>
+  <si>
+    <t>implement str Str()</t>
+  </si>
+  <si>
+    <t>Decode ways</t>
+  </si>
+  <si>
+    <t xml:space="preserve">learn about inport and export in html </t>
+  </si>
+  <si>
+    <t>PS-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">189.Rotate an Array </t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Brute-Force</t>
+  </si>
+  <si>
+    <t>PS-9</t>
+  </si>
+  <si>
+    <t>33.Search in Rotated sorted  Array</t>
+  </si>
+  <si>
+    <t>TrapicRainWater</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,18 +434,23 @@
     </font>
     <font>
       <b/>
-      <sz val="20"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Rime"/>
     </font>
   </fonts>
   <fills count="9">
@@ -392,12 +498,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -415,15 +521,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -457,13 +554,17 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color theme="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color theme="1"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -471,7 +572,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -504,23 +605,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -529,53 +613,57 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -919,13 +1007,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E127"/>
+  <dimension ref="A1:E126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.6640625" style="2" bestFit="1" customWidth="1"/>
@@ -935,7 +1023,7 @@
     <col min="6" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="21">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -952,7 +1040,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="4">
         <f>ROW()-ROW($A$2)</f>
         <v>0</v>
@@ -964,20 +1052,22 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
       <c r="B3" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="4">
         <f t="shared" ref="A4:A20" si="0">ROW()-ROW($A$2)</f>
         <v>2</v>
@@ -995,7 +1085,7 @@
         <v>45950</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1013,7 +1103,7 @@
         <v>45950</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1031,7 +1121,7 @@
         <v>45952</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1047,7 +1137,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1059,7 +1149,7 @@
       <c r="D8" s="4"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1071,7 +1161,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1083,7 +1173,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1095,7 +1185,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1107,8 +1197,10 @@
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4">
+        <v>11</v>
+      </c>
       <c r="B13" s="7" t="s">
         <v>76</v>
       </c>
@@ -1116,7 +1208,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1128,7 +1220,7 @@
       <c r="D14" s="4"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1140,7 +1232,7 @@
       <c r="D15" s="4"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1152,7 +1244,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1164,7 +1256,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1176,7 +1268,7 @@
       <c r="D18" s="5"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19" s="4">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1188,7 +1280,7 @@
       <c r="D19" s="5"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5">
       <c r="A20" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1200,7 +1292,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21" s="4">
         <f>IF(B21&lt;&gt;"", COUNTIF($B$2:B21,"&lt;&gt;"), "")</f>
         <v>20</v>
@@ -1212,7 +1304,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5">
       <c r="A22" s="4">
         <f>IF(B22&lt;&gt;"", COUNTIF($B$2:B22,"&lt;&gt;"), "")</f>
         <v>21</v>
@@ -1224,7 +1316,7 @@
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5">
       <c r="A23" s="4">
         <f>IF(B23&lt;&gt;"", COUNTIF($B$2:B23,"&lt;&gt;"), "")</f>
         <v>22</v>
@@ -1236,697 +1328,686 @@
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="str">
-        <f>IF(B24&lt;&gt;"", COUNTIF($B$2:B24,"&lt;&gt;"), "")</f>
-        <v/>
-      </c>
-      <c r="B24" s="5"/>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5">
       <c r="A25" s="4">
         <f>IF(B25&lt;&gt;"", COUNTIF($B$2:B25,"&lt;&gt;"), "")</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5">
       <c r="A26" s="4">
         <f>IF(B26&lt;&gt;"", COUNTIF($B$2:B26,"&lt;&gt;"), "")</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5">
       <c r="A27" s="4">
         <f>IF(B27&lt;&gt;"", COUNTIF($B$2:B27,"&lt;&gt;"), "")</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5">
       <c r="A28" s="4">
         <f>IF(B28&lt;&gt;"", COUNTIF($B$2:B28,"&lt;&gt;"), "")</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5">
       <c r="A29" s="4">
         <f>IF(B29&lt;&gt;"", COUNTIF($B$2:B29,"&lt;&gt;"), "")</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5">
       <c r="A30" s="4">
         <f>IF(B30&lt;&gt;"", COUNTIF($B$2:B30,"&lt;&gt;"), "")</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5">
       <c r="A31" s="4">
         <f>IF(B31&lt;&gt;"", COUNTIF($B$2:B31,"&lt;&gt;"), "")</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5">
       <c r="A32" s="4">
         <f>IF(B32&lt;&gt;"", COUNTIF($B$2:B32,"&lt;&gt;"), "")</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5">
       <c r="A33" s="4">
         <f>IF(B33&lt;&gt;"", COUNTIF($B$2:B33,"&lt;&gt;"), "")</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="21">
       <c r="A34" s="4">
         <f>IF(B34&lt;&gt;"", COUNTIF($B$2:B34,"&lt;&gt;"), "")</f>
-        <v>32</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>22</v>
+        <v>33</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5">
       <c r="A35" s="4">
         <f>IF(B35&lt;&gt;"", COUNTIF($B$2:B35,"&lt;&gt;"), "")</f>
-        <v>33</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>23</v>
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5">
       <c r="A36" s="4">
         <f>IF(B36&lt;&gt;"", COUNTIF($B$2:B36,"&lt;&gt;"), "")</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5">
       <c r="A37" s="4">
         <f>IF(B37&lt;&gt;"", COUNTIF($B$2:B37,"&lt;&gt;"), "")</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="28.8">
       <c r="A38" s="4">
         <f>IF(B38&lt;&gt;"", COUNTIF($B$2:B38,"&lt;&gt;"), "")</f>
-        <v>36</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>26</v>
+        <v>37</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
     </row>
-    <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5">
       <c r="A39" s="4">
         <f>IF(B39&lt;&gt;"", COUNTIF($B$2:B39,"&lt;&gt;"), "")</f>
-        <v>37</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>27</v>
+        <v>38</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5">
       <c r="A40" s="4">
         <f>IF(B40&lt;&gt;"", COUNTIF($B$2:B40,"&lt;&gt;"), "")</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="43.2">
       <c r="A41" s="4">
         <f>IF(B41&lt;&gt;"", COUNTIF($B$2:B41,"&lt;&gt;"), "")</f>
-        <v>39</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5">
       <c r="A42" s="4">
         <f>IF(B42&lt;&gt;"", COUNTIF($B$2:B42,"&lt;&gt;"), "")</f>
-        <v>40</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>30</v>
+        <v>41</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="4">
-        <f>IF(B43&lt;&gt;"", COUNTIF($B$2:B43,"&lt;&gt;"), "")</f>
-        <v>41</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>31</v>
+    <row r="43" spans="1:5">
+      <c r="A43" s="4"/>
+      <c r="B43" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="4"/>
-      <c r="B44" s="11" t="s">
-        <v>32</v>
-      </c>
+    <row r="44" spans="1:5">
+      <c r="A44" s="4" t="str">
+        <f>IF(B44&lt;&gt;"", COUNTA($B$2:B44), "")</f>
+        <v/>
+      </c>
+      <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="str">
-        <f>IF(B45&lt;&gt;"", COUNTA($B$2:B45), "")</f>
-        <v/>
-      </c>
+    <row r="45" spans="1:5">
+      <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="4"/>
+    <row r="46" spans="1:5">
+      <c r="A46" s="4" t="str">
+        <f>IF(B46&lt;&gt;"", COUNTA($B$2:B46), "")</f>
+        <v/>
+      </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="str">
-        <f>IF(B47&lt;&gt;"", COUNTA($B$2:B47), "")</f>
-        <v/>
-      </c>
+    <row r="47" spans="1:5">
+      <c r="A47" s="4"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="4"/>
+    <row r="48" spans="1:5">
+      <c r="A48" s="4" t="str">
+        <f>IF(B48&lt;&gt;"", COUNTA($B$2:B48), "")</f>
+        <v/>
+      </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="str">
-        <f>IF(B49&lt;&gt;"", COUNTA($B$2:B49), "")</f>
-        <v/>
-      </c>
+    <row r="49" spans="1:5">
+      <c r="A49" s="4"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="4"/>
+    <row r="50" spans="1:5">
+      <c r="A50" s="4" t="str">
+        <f>IF(B50&lt;&gt;"", COUNTA($B$2:B50), "")</f>
+        <v/>
+      </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="str">
-        <f>IF(B51&lt;&gt;"", COUNTA($B$2:B51), "")</f>
-        <v/>
-      </c>
+    <row r="51" spans="1:5">
+      <c r="A51" s="4"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="4"/>
+    <row r="52" spans="1:5">
+      <c r="A52" s="4" t="str">
+        <f>IF(B52&lt;&gt;"", COUNTA($B$2:B52), "")</f>
+        <v/>
+      </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="str">
-        <f>IF(B53&lt;&gt;"", COUNTA($B$2:B53), "")</f>
-        <v/>
-      </c>
+    <row r="53" spans="1:5">
+      <c r="A53" s="4"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="4"/>
+    <row r="54" spans="1:5">
+      <c r="A54" s="4" t="str">
+        <f>IF(B54&lt;&gt;"", COUNTA($B$2:B54), "")</f>
+        <v/>
+      </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="str">
-        <f>IF(B55&lt;&gt;"", COUNTA($B$2:B55), "")</f>
-        <v/>
-      </c>
+    <row r="55" spans="1:5">
+      <c r="A55" s="4"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="4"/>
-      <c r="B56" s="5"/>
+    <row r="56" spans="1:5">
+      <c r="A56" s="4">
+        <f>IF(B56&lt;&gt;"", COUNTA($B$2:B56), "")</f>
+        <v>43</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="4">
-        <f>IF(B57&lt;&gt;"", COUNTA($B$2:B57), "")</f>
-        <v>43</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>48</v>
-      </c>
+    <row r="57" spans="1:5">
+      <c r="A57" s="4"/>
+      <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="4"/>
+    <row r="58" spans="1:5">
+      <c r="A58" s="4" t="str">
+        <f>IF(B58&lt;&gt;"", COUNTA($B$2:B58), "")</f>
+        <v/>
+      </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="str">
-        <f>IF(B59&lt;&gt;"", COUNTA($B$2:B59), "")</f>
-        <v/>
-      </c>
+    <row r="59" spans="1:5">
+      <c r="A59" s="4"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="4"/>
+    <row r="60" spans="1:5">
+      <c r="A60" s="4" t="str">
+        <f>IF(B60&lt;&gt;"", COUNTA($B$2:B60), "")</f>
+        <v/>
+      </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="str">
-        <f>IF(B61&lt;&gt;"", COUNTA($B$2:B61), "")</f>
-        <v/>
-      </c>
+    <row r="61" spans="1:5">
+      <c r="A61" s="4"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="4"/>
+    <row r="62" spans="1:5">
+      <c r="A62" s="4" t="str">
+        <f>IF(B62&lt;&gt;"", COUNTA($B$2:B62), "")</f>
+        <v/>
+      </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="4" t="str">
-        <f>IF(B63&lt;&gt;"", COUNTA($B$2:B63), "")</f>
-        <v/>
-      </c>
+    <row r="63" spans="1:5">
+      <c r="A63" s="4"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="4"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="str">
-        <f>IF(B65&lt;&gt;"", COUNTA($B$2:B65), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="4"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="4" t="str">
-        <f>IF(B67&lt;&gt;"", COUNTA($B$2:B67), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="4"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="4" t="str">
-        <f>IF(B69&lt;&gt;"", COUNTA($B$2:B69), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="4"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="4" t="str">
-        <f>IF(B71&lt;&gt;"", COUNTA($B$2:B71), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="4"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="4" t="str">
-        <f>IF(B73&lt;&gt;"", COUNTA($B$2:B73), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="4"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="4" t="str">
-        <f>IF(B75&lt;&gt;"", COUNTA($B$2:B75), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="4"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" s="4" t="str">
-        <f>IF(B77&lt;&gt;"", COUNTA($B$2:B77), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="4"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="4" t="str">
-        <f>IF(B79&lt;&gt;"", COUNTA($B$2:B79), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="4"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="4" t="str">
-        <f>IF(B81&lt;&gt;"", COUNTA($B$2:B81), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="4"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="4" t="str">
-        <f>IF(B83&lt;&gt;"", COUNTA($B$2:B83), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="4"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="4" t="str">
-        <f>IF(B85&lt;&gt;"", COUNTA($B$2:B85), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="4"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="4" t="str">
-        <f>IF(B87&lt;&gt;"", COUNTA($B$2:B87), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" s="4"/>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" s="4" t="str">
-        <f>IF(B89&lt;&gt;"", COUNTA($B$2:B89), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" s="4"/>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" s="4" t="str">
-        <f>IF(B91&lt;&gt;"", COUNTA($B$2:B91), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" s="4"/>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" s="4" t="str">
-        <f>IF(B93&lt;&gt;"", COUNTA($B$2:B93), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" s="4"/>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" s="4" t="str">
-        <f>IF(B95&lt;&gt;"", COUNTA($B$2:B95), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" s="4"/>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" s="4" t="str">
-        <f>IF(B97&lt;&gt;"", COUNTA($B$2:B97), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" s="4"/>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" s="4" t="str">
-        <f>IF(B99&lt;&gt;"", COUNTA($B$2:B99), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" s="4"/>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" s="4" t="str">
-        <f>IF(B101&lt;&gt;"", COUNTA($B$2:B101), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" s="4"/>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" s="4" t="str">
-        <f>IF(B103&lt;&gt;"", COUNTA($B$2:B103), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" s="4"/>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" s="4" t="str">
-        <f>IF(B105&lt;&gt;"", COUNTA($B$2:B105), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106" s="4"/>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107" s="4" t="str">
-        <f>IF(B107&lt;&gt;"", COUNTA($B$2:B107), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" s="4"/>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109" s="4" t="str">
-        <f>IF(B109&lt;&gt;"", COUNTA($B$2:B109), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110" s="4"/>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111" s="4" t="str">
-        <f>IF(B111&lt;&gt;"", COUNTA($B$2:B111), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112" s="4"/>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113" s="4" t="str">
-        <f>IF(B113&lt;&gt;"", COUNTA($B$2:B113), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114" s="4"/>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115" s="4" t="str">
-        <f>IF(B115&lt;&gt;"", COUNTA($B$2:B115), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116" s="4"/>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A117" s="4" t="str">
-        <f>IF(B117&lt;&gt;"", COUNTA($B$2:B117), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118" s="4"/>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A119" s="4" t="str">
-        <f>IF(B119&lt;&gt;"", COUNTA($B$2:B119), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5">
+      <c r="A64" s="4" t="str">
+        <f>IF(B64&lt;&gt;"", COUNTA($B$2:B64), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="4"/>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="4" t="str">
+        <f>IF(B66&lt;&gt;"", COUNTA($B$2:B66), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="4"/>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="4" t="str">
+        <f>IF(B68&lt;&gt;"", COUNTA($B$2:B68), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="4"/>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="4" t="str">
+        <f>IF(B70&lt;&gt;"", COUNTA($B$2:B70), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="4"/>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="4" t="str">
+        <f>IF(B72&lt;&gt;"", COUNTA($B$2:B72), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="4"/>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="4" t="str">
+        <f>IF(B74&lt;&gt;"", COUNTA($B$2:B74), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="4"/>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="4" t="str">
+        <f>IF(B76&lt;&gt;"", COUNTA($B$2:B76), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="4"/>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="4" t="str">
+        <f>IF(B78&lt;&gt;"", COUNTA($B$2:B78), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="4"/>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="4" t="str">
+        <f>IF(B80&lt;&gt;"", COUNTA($B$2:B80), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="4"/>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="4" t="str">
+        <f>IF(B82&lt;&gt;"", COUNTA($B$2:B82), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="4"/>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="4" t="str">
+        <f>IF(B84&lt;&gt;"", COUNTA($B$2:B84), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="4"/>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="4" t="str">
+        <f>IF(B86&lt;&gt;"", COUNTA($B$2:B86), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="4"/>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="4" t="str">
+        <f>IF(B88&lt;&gt;"", COUNTA($B$2:B88), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="4"/>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="4" t="str">
+        <f>IF(B90&lt;&gt;"", COUNTA($B$2:B90), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="4"/>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="4" t="str">
+        <f>IF(B92&lt;&gt;"", COUNTA($B$2:B92), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="4"/>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="4" t="str">
+        <f>IF(B94&lt;&gt;"", COUNTA($B$2:B94), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="4"/>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="4" t="str">
+        <f>IF(B96&lt;&gt;"", COUNTA($B$2:B96), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="4"/>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="4" t="str">
+        <f>IF(B98&lt;&gt;"", COUNTA($B$2:B98), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="4"/>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="4" t="str">
+        <f>IF(B100&lt;&gt;"", COUNTA($B$2:B100), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="4"/>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="4" t="str">
+        <f>IF(B102&lt;&gt;"", COUNTA($B$2:B102), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="4"/>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="4" t="str">
+        <f>IF(B104&lt;&gt;"", COUNTA($B$2:B104), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="4"/>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="4" t="str">
+        <f>IF(B106&lt;&gt;"", COUNTA($B$2:B106), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="4"/>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="4" t="str">
+        <f>IF(B108&lt;&gt;"", COUNTA($B$2:B108), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="4"/>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="4" t="str">
+        <f>IF(B110&lt;&gt;"", COUNTA($B$2:B110), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="4"/>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="4" t="str">
+        <f>IF(B112&lt;&gt;"", COUNTA($B$2:B112), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="4"/>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="4" t="str">
+        <f>IF(B114&lt;&gt;"", COUNTA($B$2:B114), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="4"/>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="4" t="str">
+        <f>IF(B116&lt;&gt;"", COUNTA($B$2:B116), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="4"/>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="4" t="str">
+        <f>IF(B118&lt;&gt;"", COUNTA($B$2:B118), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="4"/>
+    </row>
+    <row r="120" spans="1:1">
       <c r="A120" s="4"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1">
       <c r="A121" s="4"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1">
       <c r="A122" s="4"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:1">
       <c r="A123" s="4"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:1">
       <c r="A124" s="4"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:1">
       <c r="A125" s="4"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:1">
       <c r="A126" s="4"/>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A127" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1939,450 +2020,451 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="20" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="31" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="19"/>
+      <c r="B1" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="3" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+    </row>
+    <row r="2" spans="1:8" ht="21">
+      <c r="A2" s="19"/>
+      <c r="B2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="23" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="19">
         <v>1</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="32"/>
-      <c r="B4" s="12">
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="29"/>
+      <c r="B4" s="19">
         <v>2</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
-      <c r="B5" s="12">
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="29"/>
+      <c r="B5" s="19">
         <v>3</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="32"/>
-      <c r="B6" s="12">
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="29"/>
+      <c r="B6" s="19">
         <v>4</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="12">
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="29"/>
+      <c r="B7" s="19">
         <v>5</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="32"/>
-      <c r="B8" s="12">
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="29"/>
+      <c r="B8" s="19">
         <v>6</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="12">
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="29"/>
+      <c r="B9" s="19">
         <v>7</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
-      <c r="B10" s="12">
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="29"/>
+      <c r="B10" s="19">
         <v>8</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="32"/>
-      <c r="B11" s="12">
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="29"/>
+      <c r="B11" s="19">
         <v>9</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
-      <c r="B12" s="12">
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="29"/>
+      <c r="B12" s="19">
         <v>10</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="33" t="s">
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="19">
         <v>11</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="12"/>
-      <c r="G13" t="s">
+      <c r="F13" s="19"/>
+      <c r="G13" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="20" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="34"/>
-      <c r="B14" s="12">
+    <row r="14" spans="1:8">
+      <c r="A14" s="28"/>
+      <c r="B14" s="19">
         <v>12</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" t="s">
+      <c r="F14" s="19"/>
+      <c r="G14" s="20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="35" t="s">
+    <row r="15" spans="1:8" ht="21.6" customHeight="1">
+      <c r="A15" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="19">
         <v>13</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
-      <c r="B16" s="12">
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="29"/>
+      <c r="B16" s="19">
         <v>14</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="36"/>
-      <c r="B17" s="12">
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="29"/>
+      <c r="B17" s="19">
         <v>15</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="36"/>
-      <c r="B18" s="12">
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="29"/>
+      <c r="B18" s="19">
         <v>16</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="37"/>
-      <c r="B19" s="12">
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="29"/>
+      <c r="B19" s="19">
         <v>17</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="12">
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="26"/>
+      <c r="B20" s="19">
         <v>18</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
-      <c r="B21" s="12">
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="26"/>
+      <c r="B21" s="19">
         <v>19</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
-      <c r="B22" s="12">
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="26"/>
+      <c r="B22" s="19">
         <v>20</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="18"/>
-      <c r="B23" s="12">
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="26"/>
+      <c r="B23" s="19">
         <v>21</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="18"/>
-      <c r="B24" s="12">
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="26"/>
+      <c r="B24" s="19">
         <v>22</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
-      <c r="B25" s="12">
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="19"/>
+      <c r="B25" s="19">
         <v>23</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
-      <c r="B26" s="12">
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="19"/>
+      <c r="B26" s="19">
         <v>24</v>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
-      <c r="B27" s="12">
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="19"/>
+      <c r="B27" s="19">
         <v>25</v>
       </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
-      <c r="B28" s="12">
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="19"/>
+      <c r="B28" s="19">
         <v>26</v>
       </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
-      <c r="B29" s="12">
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="19"/>
+      <c r="B29" s="19">
         <v>27</v>
       </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
-      <c r="B30" s="12">
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="19"/>
+      <c r="B30" s="19">
         <v>28</v>
       </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
-      <c r="B31" s="12">
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="19"/>
+      <c r="B31" s="19">
         <v>29</v>
       </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
-      <c r="B32" s="12">
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="19"/>
+      <c r="B32" s="19">
         <v>30</v>
       </c>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="13"/>
-      <c r="B33" s="12">
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="19"/>
+      <c r="B33" s="19">
         <v>31</v>
       </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="13"/>
-      <c r="B34" s="12">
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="19"/>
+      <c r="B34" s="19">
         <v>32</v>
       </c>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="13"/>
-      <c r="B35" s="12">
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="19"/>
+      <c r="B35" s="19">
         <v>33</v>
       </c>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
-      <c r="B36" s="12">
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="19"/>
+      <c r="B36" s="19">
         <v>34</v>
       </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="13"/>
-      <c r="B37" s="12">
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="19"/>
+      <c r="B37" s="19">
         <v>35</v>
       </c>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2403,130 +2485,150 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{411E8094-7561-49CA-9B8A-276DDABAA03D}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="40.77734375" style="19"/>
+    <col min="1" max="1" width="9.77734375" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.88671875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="40.77734375" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="25" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="23"/>
-      <c r="B1" s="23" t="s">
+    <row r="1" spans="1:7" s="36" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A1" s="34"/>
+      <c r="B1" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="36" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="29" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-    </row>
-    <row r="3" spans="1:7" s="29" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="26"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-    </row>
-    <row r="4" spans="1:7" s="29" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-    </row>
-    <row r="5" spans="1:7" s="29" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="26"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-    </row>
-    <row r="6" spans="1:7" s="29" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="26"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-    </row>
-    <row r="7" spans="1:7" s="29" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
+    <row r="2" spans="1:7" ht="20.399999999999999" customHeight="1">
+      <c r="A2" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="13">
+        <v>1</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="15">
+        <v>46064</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20.399999999999999" customHeight="1">
+      <c r="A3" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" ht="20.399999999999999" customHeight="1">
+      <c r="A4" s="32"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" ht="20.399999999999999" customHeight="1">
+      <c r="A5" s="32"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" ht="20.399999999999999" customHeight="1">
+      <c r="A6" s="32"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A7" s="32"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="13">
         <v>11</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="15">
         <v>45962</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="39"/>
-      <c r="B9" s="20">
+    <row r="9" spans="1:7">
+      <c r="A9" s="31"/>
+      <c r="B9" s="13">
         <v>12</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="19" t="s">
+      <c r="F9" s="13"/>
+      <c r="G9" s="12" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2535,9 +2637,207 @@
     <mergeCell ref="A8:A9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C8" r:id="rId1" display="https://leetcode.com/problems/powx-n/" xr:uid="{E0FE6C78-D09F-4014-957F-4F909DF7EB59}"/>
-    <hyperlink ref="C9" r:id="rId2" display="https://leetcode.com/problems/subsets/" xr:uid="{5C51491E-CCDD-4B6F-B542-2A72F22C4408}"/>
+    <hyperlink ref="C9" r:id="rId1" display="https://leetcode.com/problems/subsets/" xr:uid="{5C51491E-CCDD-4B6F-B542-2A72F22C4408}"/>
+    <hyperlink ref="C8" r:id="rId2" display="https://leetcode.com/problems/powx-n/" xr:uid="{E0FE6C78-D09F-4014-957F-4F909DF7EB59}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D574BF-1D59-4246-B6B2-8010EAAEC622}">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="42.88671875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="45.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="46.88671875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="16" customFormat="1" ht="22.8">
+      <c r="A1" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="18" customFormat="1">
+      <c r="A2" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="1:6" s="18" customFormat="1">
+      <c r="A3" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="1:6" s="18" customFormat="1">
+      <c r="A4" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:6" s="18" customFormat="1">
+      <c r="A5" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:6" s="18" customFormat="1">
+      <c r="A6" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="1:6" s="18" customFormat="1">
+      <c r="A7" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" spans="1:6" s="18" customFormat="1">
+      <c r="A8" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:6" s="18" customFormat="1">
+      <c r="A9" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="1:6" s="18" customFormat="1">
+      <c r="A10" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" s="18" customFormat="1">
+      <c r="A11" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" spans="1:6" s="18" customFormat="1"/>
+    <row r="13" spans="1:6" s="18" customFormat="1"/>
+    <row r="14" spans="1:6" s="18" customFormat="1"/>
+    <row r="15" spans="1:6" s="18" customFormat="1"/>
+    <row r="16" spans="1:6" s="18" customFormat="1"/>
+    <row r="17" spans="1:1" s="18" customFormat="1"/>
+    <row r="23" spans="1:1">
+      <c r="A23" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17B08AD3-4B0B-42F4-95F8-DA16B54040BD}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="40.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
isma excel sheet ko modify kiye hai or code me kuch vher char kiye hai
</commit_message>
<xml_diff>
--- a/Progress Tracking.xlsx
+++ b/Progress Tracking.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA-JAVA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2.Sigma 4.0\DSA-JAVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A113270-1606-4ED6-8317-0A0E2A0E5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2BDDD6-8AE3-4306-AC34-4B42F456C742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{74DA7082-15CB-48A2-8E86-E4786E99D695}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{74DA7082-15CB-48A2-8E86-E4786E99D695}"/>
   </bookViews>
   <sheets>
     <sheet name="Self Practic" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Live-Session" sheetId="3" r:id="rId3"/>
     <sheet name="Important Problem-Topic Wise" sheetId="4" r:id="rId4"/>
     <sheet name="REACT Dev" sheetId="5" r:id="rId5"/>
+    <sheet name="Easy-Level" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="116">
   <si>
     <t>Problem</t>
   </si>
@@ -378,6 +379,18 @@
   </si>
   <si>
     <t>TrapicRainWater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">problem </t>
+  </si>
+  <si>
+    <t>ps-10</t>
+  </si>
+  <si>
+    <t>med</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two pointer </t>
   </si>
 </sst>
 </file>
@@ -503,7 +516,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -528,32 +541,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color theme="1"/>
       </left>
       <right style="thin">
@@ -564,6 +551,19 @@
       </top>
       <bottom style="thin">
         <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -606,57 +606,32 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -664,6 +639,27 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1009,8 +1005,8 @@
   </sheetPr>
   <dimension ref="A1:E126"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
@@ -2020,451 +2016,471 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="20" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="20"/>
+    <col min="1" max="1" width="12.109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="17" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="19"/>
-      <c r="B1" s="28" t="s">
+      <c r="A1" s="16"/>
+      <c r="B1" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:8" ht="21">
-      <c r="A2" s="19"/>
-      <c r="B2" s="21" t="s">
+      <c r="A2" s="16"/>
+      <c r="B2" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="20" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="16">
         <v>1</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="29"/>
-      <c r="B4" s="19">
+      <c r="A4" s="36"/>
+      <c r="B4" s="16">
         <v>2</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="29"/>
-      <c r="B5" s="19">
+      <c r="A5" s="36"/>
+      <c r="B5" s="16">
         <v>3</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="29"/>
-      <c r="B6" s="19">
+      <c r="A6" s="36"/>
+      <c r="B6" s="16">
         <v>4</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="29"/>
-      <c r="B7" s="19">
+      <c r="A7" s="36"/>
+      <c r="B7" s="16">
         <v>5</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="29"/>
-      <c r="B8" s="19">
+      <c r="A8" s="36"/>
+      <c r="B8" s="16">
         <v>6</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="29"/>
-      <c r="B9" s="19">
+      <c r="A9" s="36"/>
+      <c r="B9" s="16">
         <v>7</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="29"/>
-      <c r="B10" s="19">
+      <c r="A10" s="36"/>
+      <c r="B10" s="16">
         <v>8</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="16"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="29"/>
-      <c r="B11" s="19">
+      <c r="A11" s="36"/>
+      <c r="B11" s="16">
         <v>9</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="16"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="29"/>
-      <c r="B12" s="19">
+      <c r="A12" s="36"/>
+      <c r="B12" s="16">
         <v>10</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="16"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="16">
         <v>11</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="20" t="s">
+      <c r="F13" s="16"/>
+      <c r="G13" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="28"/>
-      <c r="B14" s="19">
+      <c r="A14" s="35"/>
+      <c r="B14" s="16">
         <v>12</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="20" t="s">
+      <c r="F14" s="16"/>
+      <c r="G14" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="21.6" customHeight="1">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="16">
         <v>13</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="29"/>
-      <c r="B16" s="19">
+      <c r="A16" s="36"/>
+      <c r="B16" s="16">
         <v>14</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="29"/>
-      <c r="B17" s="19">
+      <c r="A17" s="36"/>
+      <c r="B17" s="16">
         <v>15</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="29"/>
-      <c r="B18" s="19">
+      <c r="A18" s="36"/>
+      <c r="B18" s="16">
         <v>16</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="29"/>
-      <c r="B19" s="19">
+      <c r="A19" s="36"/>
+      <c r="B19" s="16">
         <v>17</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="26"/>
-      <c r="B20" s="19">
+      <c r="A20" s="23"/>
+      <c r="B20" s="16">
         <v>18</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="26"/>
-      <c r="B21" s="19">
+      <c r="A21" s="23"/>
+      <c r="B21" s="16">
         <v>19</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="26"/>
-      <c r="B22" s="19">
+      <c r="A22" s="23"/>
+      <c r="B22" s="16">
         <v>20</v>
       </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="26"/>
-      <c r="B23" s="19">
+      <c r="A23" s="23"/>
+      <c r="B23" s="16">
         <v>21</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="26"/>
-      <c r="B24" s="19">
+      <c r="A24" s="23"/>
+      <c r="B24" s="16">
         <v>22</v>
       </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16">
         <v>23</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16">
         <v>24</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="19"/>
-      <c r="B27" s="19">
+      <c r="A27" s="16"/>
+      <c r="B27" s="16">
         <v>25</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16">
         <v>26</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19">
+      <c r="A29" s="16"/>
+      <c r="B29" s="16">
         <v>27</v>
       </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19">
+      <c r="A30" s="16"/>
+      <c r="B30" s="16">
         <v>28</v>
       </c>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19">
+      <c r="A31" s="16"/>
+      <c r="B31" s="16">
         <v>29</v>
       </c>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19">
+      <c r="A32" s="16"/>
+      <c r="B32" s="16">
         <v>30</v>
       </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19">
+      <c r="A33" s="16"/>
+      <c r="B33" s="16">
         <v>31</v>
       </c>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="19"/>
-      <c r="B34" s="19">
+      <c r="A34" s="16"/>
+      <c r="B34" s="16">
         <v>32</v>
       </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="19"/>
-      <c r="B35" s="19">
+      <c r="A35" s="16"/>
+      <c r="B35" s="16">
         <v>33</v>
       </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="19"/>
-      <c r="B36" s="19">
+      <c r="A36" s="16"/>
+      <c r="B36" s="16">
         <v>34</v>
       </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="19"/>
-      <c r="B37" s="19">
+      <c r="A37" s="16"/>
+      <c r="B37" s="16">
         <v>35</v>
       </c>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2483,10 +2499,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{411E8094-7561-49CA-9B8A-276DDABAA03D}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="15.6"/>
@@ -2501,136 +2517,278 @@
     <col min="8" max="16384" width="40.77734375" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="36" customFormat="1" ht="19.95" customHeight="1">
-      <c r="A1" s="34"/>
-      <c r="B1" s="34" t="s">
+    <row r="1" spans="1:8" s="27" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A1" s="25"/>
+      <c r="B1" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="27" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="20.399999999999999" customHeight="1">
-      <c r="A2" s="32" t="s">
+      <c r="H1" s="29"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.399999999999999" customHeight="1">
+      <c r="A2" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="28">
         <v>1</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="31">
         <v>46064</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="20.399999999999999" customHeight="1">
-      <c r="A3" s="32" t="s">
+      <c r="G2" s="32"/>
+    </row>
+    <row r="3" spans="1:8" ht="20.399999999999999" customHeight="1">
+      <c r="A3" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="33" t="s">
+      <c r="B3" s="28">
+        <v>2</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-    </row>
-    <row r="4" spans="1:7" ht="20.399999999999999" customHeight="1">
-      <c r="A4" s="32"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="33" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="32"/>
+    </row>
+    <row r="4" spans="1:8" ht="20.399999999999999" customHeight="1">
+      <c r="A4" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="28">
+        <v>3</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="1:7" ht="20.399999999999999" customHeight="1">
-      <c r="A5" s="32"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="1:7" ht="20.399999999999999" customHeight="1">
-      <c r="A6" s="32"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="1:7" ht="19.95" customHeight="1">
-      <c r="A7" s="32"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="30" t="s">
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="32"/>
+    </row>
+    <row r="5" spans="1:8" ht="20.399999999999999" customHeight="1">
+      <c r="A5" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="28">
+        <v>4</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="31">
+        <v>46069</v>
+      </c>
+      <c r="G5" s="32"/>
+    </row>
+    <row r="6" spans="1:8" ht="20.399999999999999" customHeight="1">
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="32"/>
+    </row>
+    <row r="7" spans="1:8" ht="19.95" customHeight="1">
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="32"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="28">
         <v>11</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="31">
         <v>45962</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="32" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="31"/>
-      <c r="B9" s="13">
+    <row r="9" spans="1:8">
+      <c r="A9" s="34"/>
+      <c r="B9" s="28">
         <v>12</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="12" t="s">
+      <c r="F9" s="28"/>
+      <c r="G9" s="32" t="s">
         <v>64</v>
       </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2663,148 +2821,148 @@
     <col min="7" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="16" customFormat="1" ht="22.8">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:6" s="13" customFormat="1" ht="22.8">
+      <c r="A1" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="18" customFormat="1">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:6" s="15" customFormat="1">
+      <c r="A2" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-    </row>
-    <row r="3" spans="1:6" s="18" customFormat="1">
-      <c r="A3" s="17" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:6" s="15" customFormat="1">
+      <c r="A3" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-    </row>
-    <row r="4" spans="1:6" s="18" customFormat="1">
-      <c r="A4" s="17" t="s">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:6" s="15" customFormat="1">
+      <c r="A4" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-    </row>
-    <row r="5" spans="1:6" s="18" customFormat="1">
-      <c r="A5" s="17" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:6" s="15" customFormat="1">
+      <c r="A5" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-    </row>
-    <row r="6" spans="1:6" s="18" customFormat="1">
-      <c r="A6" s="17" t="s">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:6" s="15" customFormat="1">
+      <c r="A6" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-    </row>
-    <row r="7" spans="1:6" s="18" customFormat="1">
-      <c r="A7" s="17" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:6" s="15" customFormat="1">
+      <c r="A7" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-    </row>
-    <row r="8" spans="1:6" s="18" customFormat="1">
-      <c r="A8" s="17" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:6" s="15" customFormat="1">
+      <c r="A8" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-    </row>
-    <row r="9" spans="1:6" s="18" customFormat="1">
-      <c r="A9" s="17" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" s="15" customFormat="1">
+      <c r="A9" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-    </row>
-    <row r="10" spans="1:6" s="18" customFormat="1">
-      <c r="A10" s="17" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:6" s="15" customFormat="1">
+      <c r="A10" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-    </row>
-    <row r="11" spans="1:6" s="18" customFormat="1">
-      <c r="A11" s="17" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:6" s="15" customFormat="1">
+      <c r="A11" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-    </row>
-    <row r="12" spans="1:6" s="18" customFormat="1"/>
-    <row r="13" spans="1:6" s="18" customFormat="1"/>
-    <row r="14" spans="1:6" s="18" customFormat="1"/>
-    <row r="15" spans="1:6" s="18" customFormat="1"/>
-    <row r="16" spans="1:6" s="18" customFormat="1"/>
-    <row r="17" spans="1:1" s="18" customFormat="1"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:6" s="15" customFormat="1"/>
+    <row r="13" spans="1:6" s="15" customFormat="1"/>
+    <row r="14" spans="1:6" s="15" customFormat="1"/>
+    <row r="15" spans="1:6" s="15" customFormat="1"/>
+    <row r="16" spans="1:6" s="15" customFormat="1"/>
+    <row r="17" spans="1:1" s="15" customFormat="1"/>
     <row r="23" spans="1:1">
       <c r="A23" s="7" t="s">
         <v>89</v>
@@ -2820,7 +2978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17B08AD3-4B0B-42F4-95F8-DA16B54040BD}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2835,9 +2993,666 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="27"/>
+      <c r="A2" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{087B83EA-1B4A-404F-B791-E267C946B1E4}">
+  <dimension ref="A1:B127"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="28">
+        <v>1</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="28">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="28">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="28">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="28">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="28">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="28">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="28">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="28">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="28">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="28">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="28">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="28">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="28">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="28">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="28">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="28">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="28">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="28">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="28">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="28">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="28">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="28">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="28">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="28">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="28">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="28">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="28">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="28">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="28">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="28">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="28">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="28">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="28">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="28">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="28">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="28">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="28">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="28">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="28">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="28">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="28">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="28">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="28">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="28">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="28">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="28">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="28">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="28">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="28">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="28">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="28">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="28">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="28">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="28">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="28">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="28">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="28">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="28">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="28">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="28">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="28">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="28">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="28">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="28">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="28">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="28">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="28">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="28">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="28">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="28">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="28">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="28">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="28">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="28">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="28">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="28">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="28">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="28">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="28">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="28">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="28">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="28">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="28">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="28">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="28">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="28">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="28">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="28">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="28">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="28">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="28">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="28">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="28">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="28">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="28">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="28">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="28">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="28">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="28">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="28">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="28">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="28">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="28">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="28">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="28">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="28">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
valid anagram in string toppic
</commit_message>
<xml_diff>
--- a/Progress Tracking.xlsx
+++ b/Progress Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2.Sigma 4.0\DSA-JAVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF2285D-F3DF-4530-8DC4-460AD79E0DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F309BF-4155-4151-A7D9-BBE453169667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{74DA7082-15CB-48A2-8E86-E4786E99D695}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="126">
   <si>
     <t>Problem</t>
   </si>
@@ -409,13 +409,25 @@
   </si>
   <si>
     <t>240. Search a 2D Matrix II</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>242. Valid Anagram</t>
+  </si>
+  <si>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>Brute Force,Hash map, without using space</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,6 +499,21 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -667,7 +694,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -769,16 +796,25 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2138,19 +2174,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81AFF73C-296A-4808-96EA-C6E7B73EEBD1}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="102" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="102" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A15" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="16" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.6640625" style="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="16" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="15" style="16" customWidth="1"/>
+    <col min="7" max="7" width="37.77734375" style="16" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="16"/>
   </cols>
   <sheetData>
@@ -2182,7 +2218,9 @@
       <c r="F2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="32"/>
+      <c r="G2" s="32" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="15.6">
       <c r="A3" s="41" t="s">
@@ -2452,15 +2490,15 @@
       <c r="G19" s="32"/>
     </row>
     <row r="20" spans="1:7" ht="28.2" customHeight="1">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="47"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="51"/>
     </row>
     <row r="21" spans="1:7" ht="16.2" customHeight="1">
       <c r="A21" s="31"/>
@@ -2582,27 +2620,37 @@
       <c r="F28" s="29"/>
       <c r="G28" s="32"/>
     </row>
-    <row r="29" spans="1:7" ht="15.6">
-      <c r="A29" s="29"/>
-      <c r="B29" s="29">
-        <v>27</v>
-      </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="32"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.6">
+    <row r="29" spans="1:7" ht="39" customHeight="1">
+      <c r="A29" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" s="48"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="49"/>
+    </row>
+    <row r="30" spans="1:7" ht="28.2" customHeight="1">
       <c r="A30" s="29"/>
       <c r="B30" s="29">
         <v>28</v>
       </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="32"/>
+      <c r="C30" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="34">
+        <v>46079</v>
+      </c>
+      <c r="G30" s="32" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="15.6">
       <c r="A31" s="29"/>
@@ -2691,7 +2739,8 @@
       <c r="G38" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A29:G29"/>
     <mergeCell ref="A3:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A19"/>
@@ -2707,8 +2756,11 @@
     <hyperlink ref="C24" r:id="rId6" display="https://leetcode.com/problems/search-a-2d-matrix/" xr:uid="{A73A8190-843C-4344-B8D3-AA78441B3AC5}"/>
     <hyperlink ref="C25" r:id="rId7" display="https://leetcode.com/problems/median-of-two-sorted-arrays/" xr:uid="{2110002A-B10C-4990-8B78-285061BB92AE}"/>
     <hyperlink ref="C26" r:id="rId8" display="https://leetcode.com/problems/search-a-2d-matrix-ii/" xr:uid="{C8DBBFD8-514D-40B3-B421-F81840312883}"/>
+    <hyperlink ref="C30" r:id="rId9" display="https://leetcode.com/problems/valid-anagram/" xr:uid="{31CB7D5C-0B81-4EC8-8C8B-4CF90671FBF4}"/>
   </hyperlinks>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -2847,7 +2899,7 @@
       <c r="G7" s="26"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="45" t="s">
         <v>60</v>
       </c>
       <c r="B8" s="22">
@@ -2870,7 +2922,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="48"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="22">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
bit operation code and update excel sheet
</commit_message>
<xml_diff>
--- a/Progress Tracking.xlsx
+++ b/Progress Tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2.Sigma 4.0\DSA-JAVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F309BF-4155-4151-A7D9-BBE453169667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B433B0-8A6C-478F-AF80-0B515080FA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{74DA7082-15CB-48A2-8E86-E4786E99D695}"/>
+    <workbookView xWindow="1320" yWindow="948" windowWidth="21600" windowHeight="11292" firstSheet="1" activeTab="1" xr2:uid="{74DA7082-15CB-48A2-8E86-E4786E99D695}"/>
   </bookViews>
   <sheets>
     <sheet name="Self Practic" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="131">
   <si>
     <t>Problem</t>
   </si>
@@ -421,6 +421,21 @@
   </si>
   <si>
     <t>Brute Force,Hash map, without using space</t>
+  </si>
+  <si>
+    <t>Bit Manuplation [01-03-2026]</t>
+  </si>
+  <si>
+    <t>136. Single Number</t>
+  </si>
+  <si>
+    <t>BitManuplation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">easy </t>
+  </si>
+  <si>
+    <t>Bassic</t>
   </si>
 </sst>
 </file>
@@ -784,6 +799,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -796,25 +820,16 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2175,7 +2190,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" zoomScale="102" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A15" sqref="A1:A1048576"/>
+      <selection activeCell="G30" activeCellId="1" sqref="G33 G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2183,7 +2198,7 @@
     <col min="1" max="1" width="14.33203125" style="16" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" style="16" customWidth="1"/>
     <col min="5" max="5" width="9.88671875" style="16" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" style="16" customWidth="1"/>
     <col min="7" max="7" width="37.77734375" style="16" customWidth="1"/>
@@ -2191,15 +2206,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.8">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="47"/>
     </row>
     <row r="2" spans="1:7" ht="15.6">
       <c r="A2" s="29"/>
@@ -2223,7 +2238,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.6">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="44" t="s">
         <v>59</v>
       </c>
       <c r="B3" s="29">
@@ -2240,7 +2255,7 @@
       <c r="G3" s="32"/>
     </row>
     <row r="4" spans="1:7" ht="15.6">
-      <c r="A4" s="41"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="29">
         <v>2</v>
       </c>
@@ -2255,7 +2270,7 @@
       <c r="G4" s="32"/>
     </row>
     <row r="5" spans="1:7" ht="15.6">
-      <c r="A5" s="41"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="29">
         <v>3</v>
       </c>
@@ -2270,7 +2285,7 @@
       <c r="G5" s="32"/>
     </row>
     <row r="6" spans="1:7" ht="15.6">
-      <c r="A6" s="41"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="29">
         <v>4</v>
       </c>
@@ -2285,7 +2300,7 @@
       <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:7" ht="15.6">
-      <c r="A7" s="41"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="29">
         <v>5</v>
       </c>
@@ -2300,7 +2315,7 @@
       <c r="G7" s="32"/>
     </row>
     <row r="8" spans="1:7" ht="15.6">
-      <c r="A8" s="41"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="29">
         <v>6</v>
       </c>
@@ -2315,7 +2330,7 @@
       <c r="G8" s="32"/>
     </row>
     <row r="9" spans="1:7" ht="15.6">
-      <c r="A9" s="41"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="29">
         <v>7</v>
       </c>
@@ -2330,7 +2345,7 @@
       <c r="G9" s="32"/>
     </row>
     <row r="10" spans="1:7" ht="15.6">
-      <c r="A10" s="41"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="29">
         <v>8</v>
       </c>
@@ -2345,7 +2360,7 @@
       <c r="G10" s="32"/>
     </row>
     <row r="11" spans="1:7" ht="15.6">
-      <c r="A11" s="41"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="29">
         <v>9</v>
       </c>
@@ -2360,7 +2375,7 @@
       <c r="G11" s="32"/>
     </row>
     <row r="12" spans="1:7" ht="15.6">
-      <c r="A12" s="41"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="29">
         <v>10</v>
       </c>
@@ -2375,7 +2390,7 @@
       <c r="G12" s="32"/>
     </row>
     <row r="13" spans="1:7" ht="15.6">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="44" t="s">
         <v>60</v>
       </c>
       <c r="B13" s="29">
@@ -2396,7 +2411,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.6">
-      <c r="A14" s="41"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="29">
         <v>12</v>
       </c>
@@ -2413,7 +2428,7 @@
       <c r="G14" s="32"/>
     </row>
     <row r="15" spans="1:7" ht="21.6" customHeight="1">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="44" t="s">
         <v>59</v>
       </c>
       <c r="B15" s="29">
@@ -2430,7 +2445,7 @@
       <c r="G15" s="32"/>
     </row>
     <row r="16" spans="1:7" ht="15.6">
-      <c r="A16" s="41"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="29">
         <v>14</v>
       </c>
@@ -2445,7 +2460,7 @@
       <c r="G16" s="32"/>
     </row>
     <row r="17" spans="1:7" ht="15.6">
-      <c r="A17" s="41"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="29">
         <v>15</v>
       </c>
@@ -2460,7 +2475,7 @@
       <c r="G17" s="32"/>
     </row>
     <row r="18" spans="1:7" ht="15.6">
-      <c r="A18" s="41"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="29">
         <v>16</v>
       </c>
@@ -2475,7 +2490,7 @@
       <c r="G18" s="32"/>
     </row>
     <row r="19" spans="1:7" ht="15.6">
-      <c r="A19" s="41"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="29">
         <v>17</v>
       </c>
@@ -2490,15 +2505,15 @@
       <c r="G19" s="32"/>
     </row>
     <row r="20" spans="1:7" ht="28.2" customHeight="1">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="51"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="50"/>
     </row>
     <row r="21" spans="1:7" ht="16.2" customHeight="1">
       <c r="A21" s="31"/>
@@ -2621,15 +2636,15 @@
       <c r="G28" s="32"/>
     </row>
     <row r="29" spans="1:7" ht="39" customHeight="1">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="B29" s="48"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="49"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="43"/>
     </row>
     <row r="30" spans="1:7" ht="28.2" customHeight="1">
       <c r="A30" s="29"/>
@@ -2663,27 +2678,37 @@
       <c r="F31" s="29"/>
       <c r="G31" s="32"/>
     </row>
-    <row r="32" spans="1:7" ht="15.6">
-      <c r="A32" s="29"/>
-      <c r="B32" s="29">
-        <v>30</v>
-      </c>
-      <c r="C32" s="30"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="32"/>
+    <row r="32" spans="1:7" ht="39" customHeight="1">
+      <c r="A32" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="42"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="43"/>
     </row>
     <row r="33" spans="1:7" ht="15.6">
       <c r="A33" s="29"/>
       <c r="B33" s="29">
         <v>31</v>
       </c>
-      <c r="C33" s="30"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="32"/>
+      <c r="C33" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="F33" s="34">
+        <v>46082</v>
+      </c>
+      <c r="G33" s="32" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="15.6">
       <c r="A34" s="29"/>
@@ -2739,7 +2764,8 @@
       <c r="G38" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A32:G32"/>
     <mergeCell ref="A29:G29"/>
     <mergeCell ref="A3:A12"/>
     <mergeCell ref="A13:A14"/>
@@ -2757,10 +2783,11 @@
     <hyperlink ref="C25" r:id="rId7" display="https://leetcode.com/problems/median-of-two-sorted-arrays/" xr:uid="{2110002A-B10C-4990-8B78-285061BB92AE}"/>
     <hyperlink ref="C26" r:id="rId8" display="https://leetcode.com/problems/search-a-2d-matrix-ii/" xr:uid="{C8DBBFD8-514D-40B3-B421-F81840312883}"/>
     <hyperlink ref="C30" r:id="rId9" display="https://leetcode.com/problems/valid-anagram/" xr:uid="{31CB7D5C-0B81-4EC8-8C8B-4CF90671FBF4}"/>
+    <hyperlink ref="C33" r:id="rId10" display="https://leetcode.com/problems/single-number/" xr:uid="{59594F15-BF68-4E70-8C90-9FEBE4495F04}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -2899,7 +2926,7 @@
       <c r="G7" s="26"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="51" t="s">
         <v>60</v>
       </c>
       <c r="B8" s="22">
@@ -2922,7 +2949,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="45"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="22">
         <v>12</v>
       </c>

</xml_diff>